<commit_message>
checkpoint grupo 13; feito g13.4
</commit_message>
<xml_diff>
--- a/Data/g13.4.xlsx
+++ b/Data/g13.4.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,14 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Região</t>
@@ -392,11 +468,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D2">
-        <v>88.09875854372994</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>87.15000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -412,11 +488,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>88.91898936863468</v>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>87.86</v>
       </c>
     </row>
     <row r="4">
@@ -432,11 +508,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>87.6269256467444</v>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>88.09999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -452,11 +528,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>86.40199837580568</v>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>88.92</v>
       </c>
     </row>
     <row r="6">
@@ -472,11 +548,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>85.10970347929863</v>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>87.63</v>
       </c>
     </row>
     <row r="7">
@@ -492,11 +568,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>85.82012456093744</v>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>86.40000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -512,11 +588,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
-      </c>
-      <c r="D8">
-        <v>85.09170501959174</v>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>85.11</v>
       </c>
     </row>
     <row r="9">
@@ -532,11 +608,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>85.7680202656022</v>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>85.81999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -552,11 +628,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>87.35882739828995</v>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>85.09</v>
       </c>
     </row>
     <row r="11">
@@ -572,11 +648,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>88.85372779747212</v>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>85.77</v>
       </c>
     </row>
     <row r="12">
@@ -592,11 +668,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>88.85603969260613</v>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>87.36</v>
       </c>
     </row>
     <row r="13">
@@ -612,11 +688,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D13">
-        <v>90.6967300113522</v>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>88.84999999999999</v>
       </c>
     </row>
     <row r="14">
@@ -632,11 +708,11 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D14">
-        <v>91.29946932281176</v>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>88.86</v>
       </c>
     </row>
     <row r="15">
@@ -652,11 +728,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D15">
-        <v>92.05869818976858</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>90.7</v>
       </c>
     </row>
     <row r="16">
@@ -672,11 +748,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D16">
-        <v>91.20616836197172</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>91.3</v>
       </c>
     </row>
     <row r="17">
@@ -692,11 +768,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D17">
-        <v>91.96054185222719</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>92.06</v>
       </c>
     </row>
     <row r="18">
@@ -712,11 +788,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D18">
-        <v>92.31096399578379</v>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>91.20999999999999</v>
       </c>
     </row>
     <row r="19">
@@ -732,11 +808,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D19">
-        <v>92.59072488218143</v>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>91.95999999999999</v>
       </c>
     </row>
     <row r="20">
@@ -752,11 +828,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D20">
-        <v>92.07634205061291</v>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>92.31</v>
       </c>
     </row>
     <row r="21">
@@ -772,11 +848,11 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D21">
-        <v>93.10426800277951</v>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>92.59</v>
       </c>
     </row>
     <row r="22">
@@ -792,17 +868,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D22">
-        <v>93.63718985731164</v>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>92.08</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -812,17 +888,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D23">
-        <v>85.39254559873116</v>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>93.09999999999999</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -832,11 +908,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D24">
-        <v>86.24122476500217</v>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>93.64</v>
       </c>
     </row>
     <row r="25">
@@ -852,11 +928,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D25">
-        <v>84.21958837190678</v>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>84.55</v>
       </c>
     </row>
     <row r="26">
@@ -872,8 +948,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>85.23999999999999</v>
       </c>
     </row>
     <row r="27">
@@ -889,8 +968,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>85.39</v>
       </c>
     </row>
     <row r="28">
@@ -906,8 +988,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>86.23999999999999</v>
       </c>
     </row>
     <row r="29">
@@ -923,8 +1008,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>84.22</v>
       </c>
     </row>
     <row r="30">
@@ -940,9 +1028,10 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
-      </c>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -957,9 +1046,10 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
-      </c>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -974,9 +1064,10 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
-      </c>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -991,9 +1082,10 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1008,12 +1100,10 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D34">
-        <v>87.30259251929546</v>
-      </c>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1028,12 +1118,10 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D35">
-        <v>88.02800283174703</v>
-      </c>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1048,12 +1136,10 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D36">
-        <v>89.13957176843775</v>
-      </c>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1068,12 +1154,10 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D37">
-        <v>87.76160329045526</v>
-      </c>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1088,11 +1172,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D38">
-        <v>88.67195362505535</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>87.3</v>
       </c>
     </row>
     <row r="39">
@@ -1108,11 +1192,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D39">
-        <v>89.1498039836851</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>88.03</v>
       </c>
     </row>
     <row r="40">
@@ -1128,11 +1212,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D40">
-        <v>89.56449309852451</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>89.14</v>
       </c>
     </row>
     <row r="41">
@@ -1148,11 +1232,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D41">
-        <v>88.8911025222138</v>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>87.76000000000001</v>
       </c>
     </row>
     <row r="42">
@@ -1168,11 +1252,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D42">
-        <v>90.57060153059201</v>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>88.67</v>
       </c>
     </row>
     <row r="43">
@@ -1188,17 +1272,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
-        </is>
-      </c>
-      <c r="D43">
-        <v>91.32792385113521</v>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>89.15000000000001</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1208,17 +1292,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>01/07/2019</t>
-        </is>
-      </c>
-      <c r="D44">
-        <v>85.21897810218978</v>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>89.56</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1228,17 +1312,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
-        </is>
-      </c>
-      <c r="D45">
-        <v>85.06666666666666</v>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>88.89</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1248,17 +1332,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
-        </is>
-      </c>
-      <c r="D46">
-        <v>84.21052631578947</v>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>90.56999999999999</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1268,8 +1352,11 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>01/04/2020</t>
-        </is>
+          <t>01/07/2024</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>91.33</v>
       </c>
     </row>
     <row r="48">
@@ -1285,8 +1372,11 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>01/07/2020</t>
-        </is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>84.48</v>
       </c>
     </row>
     <row r="49">
@@ -1302,8 +1392,11 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
-        </is>
+          <t>01/04/2019</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>84.65000000000001</v>
       </c>
     </row>
     <row r="50">
@@ -1319,8 +1412,11 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
-        </is>
+          <t>01/07/2019</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>85.22</v>
       </c>
     </row>
     <row r="51">
@@ -1336,8 +1432,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>01/04/2021</t>
-        </is>
+          <t>01/10/2019</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>85.06999999999999</v>
       </c>
     </row>
     <row r="52">
@@ -1353,8 +1452,11 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>01/07/2021</t>
-        </is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>84.20999999999999</v>
       </c>
     </row>
     <row r="53">
@@ -1370,9 +1472,10 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
-        </is>
-      </c>
+          <t>01/04/2020</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1387,9 +1490,10 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
-        </is>
-      </c>
+          <t>01/07/2020</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1404,12 +1508,10 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>01/04/2022</t>
-        </is>
-      </c>
-      <c r="D55">
-        <v>87.24954462659382</v>
-      </c>
+          <t>01/10/2020</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1424,12 +1526,10 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>01/07/2022</t>
-        </is>
-      </c>
-      <c r="D56">
-        <v>87.87037037037037</v>
-      </c>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1444,12 +1544,10 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
-        </is>
-      </c>
-      <c r="D57">
-        <v>88.04744525547446</v>
-      </c>
+          <t>01/04/2021</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1464,12 +1562,10 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="D58">
-        <v>88.1740775780511</v>
-      </c>
+          <t>01/07/2021</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1484,12 +1580,10 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>01/04/2023</t>
-        </is>
-      </c>
-      <c r="D59">
-        <v>89.76303317535546</v>
-      </c>
+          <t>01/10/2021</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1504,12 +1598,10 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>01/07/2023</t>
-        </is>
-      </c>
-      <c r="D60">
-        <v>90.20332717190388</v>
-      </c>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1524,11 +1616,11 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
-        </is>
-      </c>
-      <c r="D61">
-        <v>88.70214752567693</v>
+          <t>01/04/2022</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>87.25</v>
       </c>
     </row>
     <row r="62">
@@ -1544,11 +1636,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="D62">
-        <v>89.92805755395683</v>
+          <t>01/07/2022</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>87.87</v>
       </c>
     </row>
     <row r="63">
@@ -1564,11 +1656,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>01/04/2024</t>
-        </is>
-      </c>
-      <c r="D63">
-        <v>90.95792300805729</v>
+          <t>01/10/2022</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>88.05</v>
       </c>
     </row>
     <row r="64">
@@ -1584,14 +1676,134 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>88.17</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>01/04/2023</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>89.76000000000001</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>01/07/2023</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>90.2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>01/10/2023</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>88.7</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>89.93000000000001</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>90.95999999999999</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Taxa de pessoas de 14 anos ou mais de idade, na força de trabalho, na semana de referência</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
           <t>01/07/2024</t>
         </is>
       </c>
-      <c r="D64">
-        <v>91.61462979482606</v>
+      <c r="D70" t="n">
+        <v>91.61</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>